<commit_message>
fix: Fix crash on saving on same file
</commit_message>
<xml_diff>
--- a/data/autosaved.xlsx
+++ b/data/autosaved.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Student Info</t>
   </si>
@@ -647,9 +647,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.7109375" collapsed="false"/>
-    <col min="7" max="12" bestFit="true" customWidth="true" width="3.85546875" collapsed="false"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="14" width="3.85546875" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="7" max="12" bestFit="true" customWidth="true" width="3.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="14" width="3.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat: Mark attendee on WEEK mode
</commit_message>
<xml_diff>
--- a/data/autosaved.xlsx
+++ b/data/autosaved.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>Student Info</t>
   </si>
@@ -756,6 +756,9 @@
       <c r="D4" s="8"/>
       <c r="E4" s="1"/>
       <c r="F4" s="9"/>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">

</xml_diff>